<commit_message>
deploy updates: fix login + analysis/export updates
</commit_message>
<xml_diff>
--- a/excel/输出表格.xlsx
+++ b/excel/输出表格.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21855" windowHeight="8730"/>
+    <workbookView windowWidth="20520" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -43,13 +43,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF1F1F1F"/>
-        <rFont val="Arial"/>
-        <charset val="0"/>
-      </rPr>
       <t>L7D</t>
     </r>
     <r>
@@ -58,20 +51,13 @@
         <sz val="12"/>
         <color rgb="FF1F1F1F"/>
         <rFont val="宋体"/>
-        <charset val="134"/>
+        <charset val="0"/>
       </rPr>
       <t>点击</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF1F1F1F"/>
-        <rFont val="Arial"/>
-        <charset val="0"/>
-      </rPr>
       <t>L7D</t>
     </r>
     <r>
@@ -80,20 +66,13 @@
         <sz val="12"/>
         <color rgb="FF1F1F1F"/>
         <rFont val="宋体"/>
-        <charset val="134"/>
+        <charset val="0"/>
       </rPr>
       <t>佣金</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF1F1F1F"/>
-        <rFont val="Arial"/>
-        <charset val="0"/>
-      </rPr>
       <t>L7D</t>
     </r>
     <r>
@@ -102,20 +81,13 @@
         <sz val="12"/>
         <color rgb="FF1F1F1F"/>
         <rFont val="宋体"/>
-        <charset val="134"/>
+        <charset val="0"/>
       </rPr>
       <t>花费</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF1F1F1F"/>
-        <rFont val="Arial"/>
-        <charset val="0"/>
-      </rPr>
       <t>L7D</t>
     </r>
     <r>
@@ -124,20 +96,13 @@
         <sz val="12"/>
         <color rgb="FF1F1F1F"/>
         <rFont val="宋体"/>
-        <charset val="134"/>
+        <charset val="0"/>
       </rPr>
       <t>出单天数</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF1F1F1F"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
       <t>当前</t>
     </r>
     <r>
@@ -146,20 +111,13 @@
         <sz val="12"/>
         <color rgb="FF1F1F1F"/>
         <rFont val="Arial"/>
-        <charset val="0"/>
+        <charset val="134"/>
       </rPr>
       <t>Max CPC</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF1F1F1F"/>
-        <rFont val="Arial"/>
-        <charset val="0"/>
-      </rPr>
       <t>IS Budget</t>
     </r>
     <r>
@@ -168,7 +126,7 @@
         <sz val="12"/>
         <color rgb="FF1F1F1F"/>
         <rFont val="宋体"/>
-        <charset val="134"/>
+        <charset val="0"/>
       </rPr>
       <t>丢失</t>
     </r>
@@ -308,7 +266,7 @@
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,6 +446,20 @@
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1621,8 +1593,8 @@
   <sheetPr/>
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" customHeight="1"/>

</xml_diff>